<commit_message>
added logo navbar and working on rangesliders for 2021-2023
</commit_message>
<xml_diff>
--- a/NPLF Twitter 2021.xlsx
+++ b/NPLF Twitter 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tasha/Desktop/NPLF-Dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/CS/NPLF/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1854558B-6B1C-BF4D-8A6B-FD47631B373E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2476848-6E13-2D4F-A1F7-6E214EC6DE49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{08E00A5E-42EE-0845-9D8A-F492AE305E56}"/>
+    <workbookView xWindow="19360" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{08E00A5E-42EE-0845-9D8A-F492AE305E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FE53B2-A026-7A4E-9838-FDA5B14A4048}">
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AL1"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,6 +624,550 @@
         <v>37</v>
       </c>
     </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>3333</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43931</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43932</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43933</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>116</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1.7241380000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43938</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>182</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>6.0439560000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43939</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>357</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>3.9215689999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43940</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43941</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1820</v>
+      </c>
+      <c r="D21">
+        <v>42</v>
+      </c>
+      <c r="E21">
+        <v>2.3076920000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43942</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1810</v>
+      </c>
+      <c r="D22">
+        <v>24</v>
+      </c>
+      <c r="E22">
+        <v>1.3259669999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43943</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>918</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>2.1786489999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43944</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1044</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>1.1494249999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43945</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>514</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>1.167315E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>117</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>91</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>2.1978020000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43948</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>148</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>1.3513509999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43949</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>138</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43950</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>138</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>943</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+      <c r="E31">
+        <v>2.6511130000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>603</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>1.6583750000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>148</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>6.7567599999999997E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add temp data to twitter 2021
</commit_message>
<xml_diff>
--- a/NPLF Twitter 2021.xlsx
+++ b/NPLF Twitter 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/CS/NPLF/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345425FC-5DD1-7B40-8168-14D7DEC48778}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D00BED-AF14-794A-9260-F7B93FC74A3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="1680" windowWidth="28040" windowHeight="17440" xr2:uid="{08E00A5E-42EE-0845-9D8A-F492AE305E56}"/>
+    <workbookView xWindow="280" yWindow="840" windowWidth="18740" windowHeight="17440" xr2:uid="{08E00A5E-42EE-0845-9D8A-F492AE305E56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,22 +625,124 @@
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
test temp data for twitter 2021
</commit_message>
<xml_diff>
--- a/NPLF Twitter 2021.xlsx
+++ b/NPLF Twitter 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/CS/NPLF/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D00BED-AF14-794A-9260-F7B93FC74A3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1E2FCF-A6D4-3846-A9B0-1F1A5E90AA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="840" windowWidth="18740" windowHeight="17440" xr2:uid="{08E00A5E-42EE-0845-9D8A-F492AE305E56}"/>
   </bookViews>
@@ -503,7 +503,7 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +626,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43922</v>
+        <v>44287</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43923</v>
+        <v>44288</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43924</v>
+        <v>44289</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43925</v>
+        <v>44290</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43926</v>
+        <v>44291</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43927</v>
+        <v>44292</v>
       </c>
       <c r="B7">
         <v>1</v>

</xml_diff>